<commit_message>
Fix comparing Date fields
</commit_message>
<xml_diff>
--- a/test/data/Packungen-2015.07.02.xlsx
+++ b/test/data/Packungen-2015.07.02.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="600" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="Zugelassene Packungen" sheetId="1" state="visible" r:id="rId2"/>
@@ -13,22 +13,34 @@
   <definedNames>
     <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Titles" vbProcedure="false">'Zugelassene Packungen'!$5:$5</definedName>
     <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Titles" vbProcedure="false">'Zugelassene Packungen'!$5:$5</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Titles_0" vbProcedure="false">'Zugelassene Packungen'!$5:$5</definedName>
   </definedNames>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
+  <extLst>
+    <ext xmlns:loext="http://schemas.libreoffice.org/" uri="{7626C862-2A13-11E5-B345-FEFF819CDC9F}">
+      <loext:extCalcPr stringRefSyntax="CalcA1ExcelA1"/>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="130" uniqueCount="67">
   <si>
-    <t>Zugelassene Packungen / Conditionnements autorisés</t>
-  </si>
-  <si>
-    <t>Stand / Etat au: 30.06.2015</t>
+    <t xml:space="preserve">Zugelassene Packungen / Conditionnements autorisés</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Stand / Etat au: 30.06.2015</t>
   </si>
   <si>
     <r>
-      <t>* Die Gültigkeitsdauer entspricht den Angaben auf der Zulassungsbescheinigung. Provisorische Zulassungen, ohne Erneuerung des Gültigkeitsdatums, sind vorbehalten. Alle in der Liste aufgeführten Arzneimittel sind zum Zeitpunkt der Aktualisierung der Liste zugelassen / 
+      <rPr>
+        <sz val="8.5"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">* Die Gültigkeitsdauer entspricht den Angaben auf der Zulassungsbescheinigung. Provisorische Zulassungen, ohne Erneuerung des Gültigkeitsdatums, sind vorbehalten. Alle in der Liste aufgeführten Arzneimittel sind zum Zeitpunkt der Aktualisierung der Liste zugelassen / 
   La durée de validité correspond aux données figurant sur le certificat d'autorisation. Les autorisations provisoires, sans report de la date d'expiration, restent réservées. Tous les médicaments énumérés dans la liste sont autorisés au moment de la mise à jour de la liste. 
 ** </t>
     </r>
@@ -40,7 +52,7 @@
         <family val="2"/>
         <charset val="1"/>
       </rPr>
-      <t>Verzeichnisse</t>
+      <t xml:space="preserve">Verzeichnisse</t>
     </r>
     <r>
       <rPr>
@@ -49,7 +61,7 @@
         <family val="2"/>
         <charset val="1"/>
       </rPr>
-      <t> (Kategorien der Kontrollmassnahmen, denen die Betäubungsmittel unterstellt sind) / Tableaux (catégories de mesures de contrôle auxquelles sont soumis les stupéfiants)
+      <t xml:space="preserve"> (Kategorien der Kontrollmassnahmen, denen die Betäubungsmittel unterstellt sind) / Tableaux (catégories de mesures de contrôle auxquelles sont soumis les stupéfiants)
 a: Unterstehen allen Kontrollmassnahmen (s. auch Anhang a der BetmVV-EDI) / Soumis à toutes les mesures de contrôle (voir aussi le tableau a de l'OTStup-DFI)
 b: Unterstehen nicht allen Kontrollmassnahmen (s. auch Anhang b der BetmVV-EDI) / Soustraits partiellement au contrôle (voir aussi le tableau b de l'OTStup-DFI)
 c: Unterstehen nicht allen Kontrollmassnahmen; in kleinen Mengen ohne Verschreibung erhältlich (s. auch Verzeichnis c der BetmVV-EDI) / Soustraits partiellement au contrôle; pouvant être obtenus en petites quantités sans ordonnance (voir aussi le tableau c de l'OTStup-DFI)
@@ -58,222 +70,222 @@
     </r>
   </si>
   <si>
-    <t>Zulassungs-nummer
+    <t xml:space="preserve">Zulassungs-nummer
 Numéro d'autorisation
 </t>
   </si>
   <si>
-    <t>Dosisstärke-nummer
+    <t xml:space="preserve">Dosisstärke-nummer
 Numéro de dosage</t>
   </si>
   <si>
-    <t>Präparatebezeichnung  
+    <t xml:space="preserve">Präparatebezeichnung  
 Dénomination de la préparation</t>
   </si>
   <si>
-    <t>Zulassungsinhaberin
+    <t xml:space="preserve">Zulassungsinhaberin
 Titulaire de l'autorisation</t>
   </si>
   <si>
-    <t>Heilmittelcode
+    <t xml:space="preserve">Heilmittelcode
 Catégorie de la préparation</t>
   </si>
   <si>
-    <t>IT-Nummer
+    <t xml:space="preserve">IT-Nummer
 N° IT </t>
   </si>
   <si>
-    <t>ATC-Code
+    <t xml:space="preserve">ATC-Code
 Code ATC</t>
   </si>
   <si>
-    <t>Erstzulassungs-datum Präparat
+    <t xml:space="preserve">Erstzulassungs-datum Präparat
 Date de première autorisation de la préparation</t>
   </si>
   <si>
-    <t>Zul.datum Dosisstärke 
+    <t xml:space="preserve">Zul.datum Dosisstärke 
 Date d'autorisation du dosage</t>
   </si>
   <si>
-    <t>Gültigkeitsdauer der Zulassung * 
+    <t xml:space="preserve">Gültigkeitsdauer der Zulassung * 
 Durée de validité de l'AMM  *</t>
   </si>
   <si>
-    <t>Packungscode
+    <t xml:space="preserve">Packungscode
 Code d'emballage</t>
   </si>
   <si>
-    <t>Packungsgrösse
+    <t xml:space="preserve">Packungsgrösse
 Conditionnement</t>
   </si>
   <si>
-    <t>Einheit
+    <t xml:space="preserve">Einheit
 Unité</t>
   </si>
   <si>
-    <t>Abgabekategorie Packung
+    <t xml:space="preserve">Abgabekategorie Packung
 Cat. de remise du conditionnement</t>
   </si>
   <si>
-    <t>Abgabekategorie Dosisstärke 
+    <t xml:space="preserve">Abgabekategorie Dosisstärke 
 Cat. de remise du dosage</t>
   </si>
   <si>
-    <t>Abgabekategorie Präparat
+    <t xml:space="preserve">Abgabekategorie Präparat
 Cat. de remise de la préparation</t>
   </si>
   <si>
-    <t>Wirkstoff(e)
+    <t xml:space="preserve">Wirkstoff(e)
 Principe(s) actif(s)</t>
   </si>
   <si>
-    <t>Zusammensetzung
+    <t xml:space="preserve">Zusammensetzung
 Composition</t>
   </si>
   <si>
-    <t>Anwendungsgebiet Präparat
+    <t xml:space="preserve">Anwendungsgebiet Präparat
 Champ d'application de la préparation</t>
   </si>
   <si>
-    <t>Anwendungsgebiet Dosisstärke
+    <t xml:space="preserve">Anwendungsgebiet Dosisstärke
 Champ d'application du dosage</t>
   </si>
   <si>
-    <t>Gentechnisch hergestellte Wirkstoffe
+    <t xml:space="preserve">Gentechnisch hergestellte Wirkstoffe
 Principes actifs produits par génie génétique</t>
   </si>
   <si>
-    <t>Kategorie bei Insulinen
+    <t xml:space="preserve">Kategorie bei Insulinen
 Catégorie en cas d'insuline</t>
   </si>
   <si>
-    <t>Verz. bei betäubunsmittel-haltigen Präparaten** 
+    <t xml:space="preserve">Verz. bei betäubunsmittel-haltigen Präparaten** 
 N° du tabl. si préparations à base de stupéfiants**</t>
   </si>
   <si>
-    <t>Coeur-Vaisseaux Sérocytol, suppositoire</t>
-  </si>
-  <si>
-    <t>Sérolab, société anonyme</t>
-  </si>
-  <si>
-    <t>Blutprodukte</t>
-  </si>
-  <si>
-    <t>08.07.</t>
-  </si>
-  <si>
-    <t>J06AA</t>
-  </si>
-  <si>
-    <t>3</t>
-  </si>
-  <si>
-    <t>Suppositorien</t>
-  </si>
-  <si>
-    <t>B</t>
-  </si>
-  <si>
-    <t>globulina equina (immunisé avec coeur, endothélium vasculaire porcins)</t>
-  </si>
-  <si>
-    <t>globulina equina (immunisé avec coeur, endothélium vasculaire porcins) 8 mg, propylenglycolum, conserv.: E 216, E 218, excipiens pro suppositorio.</t>
-  </si>
-  <si>
-    <t>Traitement immunomodulant selon le Dr Thomas
+    <t xml:space="preserve">Coeur-Vaisseaux Sérocytol CHANGED</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Sérolab, société anonyme</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Blutprodukte</t>
+  </si>
+  <si>
+    <t xml:space="preserve">08.07.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">J06AA</t>
+  </si>
+  <si>
+    <t xml:space="preserve">3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Suppositorien</t>
+  </si>
+  <si>
+    <t xml:space="preserve">B</t>
+  </si>
+  <si>
+    <t xml:space="preserve">globulina equina (immunisé avec coeur, endothélium vasculaire porcins)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">globulina equina (immunisé avec coeur, endothélium vasculaire porcins) 8 mg, propylenglycolum, conserv.: E 216, E 218, excipiens pro suppositorio.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Traitement immunomodulant selon le Dr Thomas
 Possibilités d'emploi voir information professionnelle</t>
   </si>
   <si>
-    <t>9</t>
-  </si>
-  <si>
-    <t>Colon Sérocytol, suppositoire</t>
-  </si>
-  <si>
-    <t>globulina equina (immunisé avec tissu intestinal porcin)</t>
-  </si>
-  <si>
-    <t>globulina equina (immunisé avec tissu intestinal porcin) 8 mg, propylenglycolum, conserv.: E 216, E 218, excipiens pro suppositorio.</t>
-  </si>
-  <si>
-    <t>Traitement immunomodulant  selon le Dr Thomas
+    <t xml:space="preserve">9</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Colon Sérocytol, suppositoire</t>
+  </si>
+  <si>
+    <t xml:space="preserve">globulina equina (immunisé avec tissu intestinal porcin)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">globulina equina (immunisé avec tissu intestinal porcin) 8 mg, propylenglycolum, conserv.: E 216, E 218, excipiens pro suppositorio.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Traitement immunomodulant  selon le Dr Thomas
 Possibilités d'emploi voir information professionnelle</t>
   </si>
   <si>
-    <t>Conjonctif Sérocytol, suppositoire</t>
-  </si>
-  <si>
-    <t>globulina equina (immunisé avec tissu conjonctif porcin)</t>
-  </si>
-  <si>
-    <t>globulina equina (immunisé avec tissu conjonctif porcin) 8 mg, propylenglycolum, conserv.: E 216, E 218, excipiens pro suppositorio.</t>
-  </si>
-  <si>
-    <t>Coop Vitality Diphenhydramin, Tabletten</t>
-  </si>
-  <si>
-    <t>Coop Vitality Health Care GmbH</t>
-  </si>
-  <si>
-    <t>Synthetika human</t>
-  </si>
-  <si>
-    <t>01.03.1.</t>
-  </si>
-  <si>
-    <t>N05CM</t>
-  </si>
-  <si>
-    <t>20</t>
-  </si>
-  <si>
-    <t>Tablette(n)</t>
-  </si>
-  <si>
-    <t>C</t>
-  </si>
-  <si>
-    <t>diphenhydramini hydrochloridum</t>
-  </si>
-  <si>
-    <t>diphenhydramini hydrochloridum 50 mg, excipiens pro compresso.</t>
-  </si>
-  <si>
-    <t>Hypnoticum</t>
-  </si>
-  <si>
-    <t>Amavita Hamamelis, Salbe</t>
-  </si>
-  <si>
-    <t>Amavita Health Care AG</t>
-  </si>
-  <si>
-    <t>Phytotherapeutika</t>
-  </si>
-  <si>
-    <t>10.06.0.</t>
-  </si>
-  <si>
-    <t>D03AX</t>
-  </si>
-  <si>
-    <t>35</t>
-  </si>
-  <si>
-    <t>g</t>
-  </si>
-  <si>
-    <t>D</t>
-  </si>
-  <si>
-    <t>hamamelidis aqua</t>
-  </si>
-  <si>
-    <t>hamamelidis aqua 150 mg, alcoholes adipis lanae, adeps lanae, conserv.: E 217, E 219, excipiens ad unguentum pro 1 g.</t>
-  </si>
-  <si>
-    <t>Bei kleineren Hautverletzungen</t>
+    <t xml:space="preserve">Conjonctif Sérocytol, suppositoire</t>
+  </si>
+  <si>
+    <t xml:space="preserve">globulina equina (immunisé avec tissu conjonctif porcin)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">globulina equina (immunisé avec tissu conjonctif porcin) 8 mg, propylenglycolum, conserv.: E 216, E 218, excipiens pro suppositorio.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Coop Vitality Diphenhydramin, Tabletten</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Coop Vitality Health Care GmbH</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Synthetika human</t>
+  </si>
+  <si>
+    <t xml:space="preserve">01.03.1.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">N05CM</t>
+  </si>
+  <si>
+    <t xml:space="preserve">20</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Tablette(n)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">C</t>
+  </si>
+  <si>
+    <t xml:space="preserve">diphenhydramini hydrochloridum</t>
+  </si>
+  <si>
+    <t xml:space="preserve">diphenhydramini hydrochloridum 50 mg, excipiens pro compresso.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Hypnoticum</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Amavita Hamamelis, Salbe</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Amavita Health Care AG</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Phytotherapeutika</t>
+  </si>
+  <si>
+    <t xml:space="preserve">10.06.0.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">D03AX</t>
+  </si>
+  <si>
+    <t xml:space="preserve">35</t>
+  </si>
+  <si>
+    <t xml:space="preserve">g</t>
+  </si>
+  <si>
+    <t xml:space="preserve">D</t>
+  </si>
+  <si>
+    <t xml:space="preserve">hamamelidis aqua</t>
+  </si>
+  <si>
+    <t xml:space="preserve">hamamelidis aqua 150 mg, alcoholes adipis lanae, adeps lanae, conserv.: E 217, E 219, excipiens ad unguentum pro 1 g.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Bei kleineren Hautverletzungen</t>
   </si>
 </sst>
 </file>
@@ -281,7 +293,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
-    <numFmt numFmtId="164" formatCode="GENERAL"/>
+    <numFmt numFmtId="164" formatCode="General"/>
     <numFmt numFmtId="165" formatCode="00000"/>
     <numFmt numFmtId="166" formatCode="DD/MM/YY;@"/>
     <numFmt numFmtId="167" formatCode="000"/>
@@ -420,7 +432,7 @@
       <protection locked="true" hidden="false"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="50">
+  <cellXfs count="44">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -453,10 +465,6 @@
       <alignment horizontal="general" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="20" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -473,10 +481,6 @@
       <alignment horizontal="center" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="166" fontId="4" fillId="0" borderId="0" xfId="20" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
     <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -485,18 +489,6 @@
       <alignment horizontal="right" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="20" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="20" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="20" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
     <xf numFmtId="165" fontId="4" fillId="0" borderId="1" xfId="20" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -553,14 +545,6 @@
       <alignment horizontal="center" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="20" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="20" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
     <xf numFmtId="164" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -611,6 +595,10 @@
     </xf>
     <xf numFmtId="167" fontId="4" fillId="0" borderId="0" xfId="20" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="165" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
@@ -629,7 +617,7 @@
     <cellStyle name="Currency" xfId="17" builtinId="4" customBuiltin="false"/>
     <cellStyle name="Currency [0]" xfId="18" builtinId="7" customBuiltin="false"/>
     <cellStyle name="Percent" xfId="19" builtinId="5" customBuiltin="false"/>
-    <cellStyle name="Standard 2" xfId="20" builtinId="54" customBuiltin="true"/>
+    <cellStyle name="Excel Built-in Standard 2" xfId="20" builtinId="53" customBuiltin="true"/>
   </cellStyles>
 </styleSheet>
 </file>
@@ -645,9 +633,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>2</xdr:col>
-      <xdr:colOff>360360</xdr:colOff>
+      <xdr:colOff>360000</xdr:colOff>
       <xdr:row>1</xdr:row>
-      <xdr:rowOff>238680</xdr:rowOff>
+      <xdr:rowOff>238320</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -661,7 +649,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="36360" y="360"/>
-          <a:ext cx="1600920" cy="504720"/>
+          <a:ext cx="1600560" cy="504360"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -681,95 +669,81 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="1:5574"/>
+  <dimension ref="A1:AMJ5574"/>
   <sheetViews>
-    <sheetView windowProtection="true" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="false" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="false" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="0" ySplit="5" topLeftCell="A6" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="A12" activeCellId="0" sqref="12:13"/>
+      <selection pane="bottomLeft" activeCell="J9" activeCellId="0" sqref="J9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.75"/>
+  <sheetFormatPr defaultRowHeight="12.75" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="9.12093023255814"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="2" width="7.37674418604651"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="3" width="33.8744186046512"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="3" width="22.9953488372093"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="3" width="15.8744186046512"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="2" width="7.87441860465116"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="2" width="8.12093023255814"/>
-    <col collapsed="false" hidden="false" max="9" min="8" style="4" width="10.2558139534884"/>
-    <col collapsed="false" hidden="false" max="10" min="10" style="4" width="10.1255813953488"/>
-    <col collapsed="false" hidden="false" max="11" min="11" style="4" width="9.25581395348837"/>
-    <col collapsed="false" hidden="false" max="12" min="12" style="2" width="11"/>
-    <col collapsed="false" hidden="false" max="13" min="13" style="2" width="11.3813953488372"/>
-    <col collapsed="false" hidden="false" max="14" min="14" style="5" width="10.3767441860465"/>
-    <col collapsed="false" hidden="false" max="15" min="15" style="6" width="10.3767441860465"/>
-    <col collapsed="false" hidden="false" max="16" min="16" style="2" width="10.3767441860465"/>
-    <col collapsed="false" hidden="false" max="18" min="17" style="3" width="22.1255813953488"/>
-    <col collapsed="false" hidden="false" max="20" min="19" style="3" width="26.3767441860465"/>
-    <col collapsed="false" hidden="false" max="22" min="21" style="2" width="16.1302325581395"/>
-    <col collapsed="false" hidden="false" max="23" min="23" style="2" width="14.1255813953488"/>
-    <col collapsed="false" hidden="false" max="27" min="25" style="7" width="7.25116279069767"/>
-    <col collapsed="false" hidden="false" max="28" min="28" style="7" width="8.37674418604651"/>
-    <col collapsed="false" hidden="false" max="29" min="29" style="7" width="7.25116279069767"/>
-    <col collapsed="false" hidden="false" max="30" min="30" style="7" width="14.2511627906977"/>
-    <col collapsed="false" hidden="false" max="31" min="31" style="7" width="7.25116279069767"/>
-    <col collapsed="false" hidden="false" max="1025" min="32" style="7" width="5.9953488372093"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="9.12"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="2" width="7.38"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="3" width="33.87"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="3" width="23"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="3" width="15.87"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="2" width="7.87"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="2" width="8.12"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="8" style="4" width="10.26"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="4" width="10.13"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="4" width="9.26"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="2" width="11"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="13" style="2" width="11.38"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="14" min="14" style="5" width="10.38"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="15" min="15" style="6" width="10.38"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="16" min="16" style="2" width="10.38"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="18" min="17" style="3" width="22.13"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="20" min="19" style="3" width="26.38"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="22" min="21" style="2" width="16.13"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="23" min="23" style="2" width="14.13"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="24" min="24" style="0" width="8.61"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="27" min="25" style="7" width="7.25"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="28" min="28" style="7" width="8.38"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="29" min="29" style="7" width="7.25"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="30" min="30" style="7" width="14.25"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="31" min="31" style="7" width="7.25"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="32" style="7" width="6"/>
   </cols>
   <sheetData>
-    <row r="1" s="16" customFormat="true" ht="21" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A1" s="8"/>
-      <c r="B1" s="9"/>
-      <c r="C1" s="10"/>
-      <c r="D1" s="10"/>
-      <c r="E1" s="11"/>
-      <c r="F1" s="12"/>
-      <c r="G1" s="8"/>
-      <c r="H1" s="13"/>
-      <c r="I1" s="14"/>
-      <c r="J1" s="14"/>
-      <c r="K1" s="8"/>
-      <c r="L1" s="8"/>
-      <c r="M1" s="9"/>
-      <c r="N1" s="8"/>
-      <c r="O1" s="15" t="s">
+    <row r="1" customFormat="false" ht="21" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A1" s="2"/>
+      <c r="B1" s="8"/>
+      <c r="C1" s="9"/>
+      <c r="D1" s="9"/>
+      <c r="E1" s="10"/>
+      <c r="F1" s="11"/>
+      <c r="I1" s="12"/>
+      <c r="J1" s="12"/>
+      <c r="K1" s="2"/>
+      <c r="M1" s="8"/>
+      <c r="N1" s="2"/>
+      <c r="O1" s="13" t="s">
         <v>0</v>
       </c>
-      <c r="Q1" s="17"/>
-      <c r="R1" s="17"/>
-      <c r="S1" s="18"/>
-      <c r="T1" s="18"/>
-      <c r="U1" s="8"/>
-      <c r="V1" s="8"/>
-      <c r="W1" s="8"/>
+      <c r="P1" s="7"/>
+      <c r="X1" s="7"/>
     </row>
     <row r="2" customFormat="false" ht="21" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A2" s="19"/>
-      <c r="B2" s="20"/>
-      <c r="C2" s="21"/>
-      <c r="D2" s="21"/>
-      <c r="E2" s="22"/>
-      <c r="F2" s="23"/>
-      <c r="G2" s="24"/>
-      <c r="H2" s="25"/>
-      <c r="I2" s="26"/>
-      <c r="J2" s="26"/>
-      <c r="K2" s="20"/>
-      <c r="L2" s="24"/>
-      <c r="M2" s="20"/>
-      <c r="N2" s="24"/>
-      <c r="O2" s="27" t="s">
+      <c r="A2" s="14"/>
+      <c r="B2" s="15"/>
+      <c r="C2" s="16"/>
+      <c r="D2" s="16"/>
+      <c r="E2" s="17"/>
+      <c r="F2" s="18"/>
+      <c r="G2" s="19"/>
+      <c r="H2" s="20"/>
+      <c r="I2" s="21"/>
+      <c r="J2" s="21"/>
+      <c r="K2" s="15"/>
+      <c r="L2" s="19"/>
+      <c r="M2" s="15"/>
+      <c r="N2" s="19"/>
+      <c r="O2" s="22" t="s">
         <v>1</v>
       </c>
       <c r="P2" s="0"/>
-      <c r="Q2" s="17"/>
-      <c r="R2" s="17"/>
-      <c r="S2" s="18"/>
-      <c r="T2" s="18"/>
-      <c r="U2" s="8"/>
-      <c r="V2" s="8"/>
-      <c r="W2" s="8"/>
       <c r="Y2" s="0"/>
       <c r="Z2" s="0"/>
       <c r="AA2" s="0"/>
@@ -1772,29 +1746,21 @@
       <c r="AMJ2" s="0"/>
     </row>
     <row r="3" customFormat="false" ht="10.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A3" s="28"/>
-      <c r="B3" s="28"/>
-      <c r="C3" s="29"/>
-      <c r="D3" s="29"/>
-      <c r="E3" s="30"/>
-      <c r="F3" s="31"/>
-      <c r="G3" s="31"/>
-      <c r="H3" s="32"/>
-      <c r="I3" s="32"/>
-      <c r="J3" s="32"/>
-      <c r="K3" s="28"/>
-      <c r="L3" s="28"/>
-      <c r="M3" s="28"/>
-      <c r="N3" s="28"/>
-      <c r="O3" s="33"/>
-      <c r="P3" s="34"/>
-      <c r="Q3" s="17"/>
-      <c r="R3" s="17"/>
-      <c r="S3" s="18"/>
-      <c r="T3" s="18"/>
-      <c r="U3" s="8"/>
-      <c r="V3" s="8"/>
-      <c r="W3" s="8"/>
+      <c r="A3" s="23"/>
+      <c r="B3" s="23"/>
+      <c r="C3" s="24"/>
+      <c r="D3" s="24"/>
+      <c r="E3" s="25"/>
+      <c r="F3" s="26"/>
+      <c r="G3" s="26"/>
+      <c r="H3" s="27"/>
+      <c r="I3" s="27"/>
+      <c r="J3" s="27"/>
+      <c r="K3" s="23"/>
+      <c r="L3" s="23"/>
+      <c r="M3" s="23"/>
+      <c r="N3" s="23"/>
+      <c r="O3" s="2"/>
       <c r="Y3" s="0"/>
       <c r="Z3" s="0"/>
       <c r="AA3" s="0"/>
@@ -2797,31 +2763,24 @@
       <c r="AMJ3" s="0"/>
     </row>
     <row r="4" customFormat="false" ht="96.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A4" s="35" t="s">
+      <c r="A4" s="28" t="s">
         <v>2</v>
       </c>
-      <c r="B4" s="35"/>
-      <c r="C4" s="35"/>
-      <c r="D4" s="35"/>
-      <c r="E4" s="35"/>
-      <c r="F4" s="35"/>
-      <c r="G4" s="35"/>
-      <c r="H4" s="35"/>
-      <c r="I4" s="35"/>
-      <c r="J4" s="35"/>
-      <c r="K4" s="35"/>
-      <c r="L4" s="35"/>
-      <c r="M4" s="35"/>
-      <c r="N4" s="35"/>
-      <c r="O4" s="35"/>
-      <c r="P4" s="36"/>
-      <c r="Q4" s="17"/>
-      <c r="R4" s="17"/>
-      <c r="S4" s="18"/>
-      <c r="T4" s="18"/>
-      <c r="U4" s="8"/>
-      <c r="V4" s="8"/>
-      <c r="W4" s="8"/>
+      <c r="B4" s="28"/>
+      <c r="C4" s="28"/>
+      <c r="D4" s="28"/>
+      <c r="E4" s="28"/>
+      <c r="F4" s="28"/>
+      <c r="G4" s="28"/>
+      <c r="H4" s="28"/>
+      <c r="I4" s="28"/>
+      <c r="J4" s="28"/>
+      <c r="K4" s="28"/>
+      <c r="L4" s="28"/>
+      <c r="M4" s="28"/>
+      <c r="N4" s="28"/>
+      <c r="O4" s="28"/>
+      <c r="P4" s="29"/>
       <c r="Y4" s="0"/>
       <c r="Z4" s="0"/>
       <c r="AA4" s="0"/>
@@ -3823,580 +3782,580 @@
       <c r="AMI4" s="0"/>
       <c r="AMJ4" s="0"/>
     </row>
-    <row r="5" s="42" customFormat="true" ht="89.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="37" t="s">
+    <row r="5" s="35" customFormat="true" ht="89.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="30" t="s">
         <v>3</v>
       </c>
-      <c r="B5" s="37" t="s">
+      <c r="B5" s="30" t="s">
         <v>4</v>
       </c>
-      <c r="C5" s="38" t="s">
+      <c r="C5" s="31" t="s">
         <v>5</v>
       </c>
-      <c r="D5" s="38" t="s">
+      <c r="D5" s="31" t="s">
         <v>6</v>
       </c>
-      <c r="E5" s="39" t="s">
+      <c r="E5" s="32" t="s">
         <v>7</v>
       </c>
-      <c r="F5" s="40" t="s">
+      <c r="F5" s="33" t="s">
         <v>8</v>
       </c>
-      <c r="G5" s="40" t="s">
+      <c r="G5" s="33" t="s">
         <v>9</v>
       </c>
-      <c r="H5" s="41" t="s">
+      <c r="H5" s="34" t="s">
         <v>10</v>
       </c>
-      <c r="I5" s="41" t="s">
+      <c r="I5" s="34" t="s">
         <v>11</v>
       </c>
-      <c r="J5" s="41" t="s">
+      <c r="J5" s="34" t="s">
         <v>12</v>
       </c>
-      <c r="K5" s="37" t="s">
+      <c r="K5" s="30" t="s">
         <v>13</v>
       </c>
-      <c r="L5" s="37" t="s">
+      <c r="L5" s="30" t="s">
         <v>14</v>
       </c>
-      <c r="M5" s="37" t="s">
+      <c r="M5" s="30" t="s">
         <v>15</v>
       </c>
-      <c r="N5" s="37" t="s">
+      <c r="N5" s="30" t="s">
         <v>16</v>
       </c>
-      <c r="O5" s="40" t="s">
+      <c r="O5" s="33" t="s">
         <v>17</v>
       </c>
-      <c r="P5" s="40" t="s">
+      <c r="P5" s="33" t="s">
         <v>18</v>
       </c>
-      <c r="Q5" s="39" t="s">
+      <c r="Q5" s="32" t="s">
         <v>19</v>
       </c>
-      <c r="R5" s="39" t="s">
+      <c r="R5" s="32" t="s">
         <v>20</v>
       </c>
-      <c r="S5" s="39" t="s">
+      <c r="S5" s="32" t="s">
         <v>21</v>
       </c>
-      <c r="T5" s="39" t="s">
+      <c r="T5" s="32" t="s">
         <v>22</v>
       </c>
-      <c r="U5" s="40" t="s">
+      <c r="U5" s="33" t="s">
         <v>23</v>
       </c>
-      <c r="V5" s="40" t="s">
+      <c r="V5" s="33" t="s">
         <v>24</v>
       </c>
-      <c r="W5" s="40" t="s">
+      <c r="W5" s="33" t="s">
         <v>25</v>
       </c>
     </row>
     <row r="6" s="7" customFormat="true" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A6" s="43" t="n">
+      <c r="A6" s="36" t="n">
         <v>277</v>
       </c>
-      <c r="B6" s="44" t="n">
+      <c r="B6" s="37" t="n">
         <v>1</v>
       </c>
-      <c r="C6" s="45" t="s">
+      <c r="C6" s="38" t="s">
         <v>26</v>
       </c>
-      <c r="D6" s="45" t="s">
+      <c r="D6" s="38" t="s">
         <v>27</v>
       </c>
-      <c r="E6" s="45" t="s">
+      <c r="E6" s="38" t="s">
         <v>28</v>
       </c>
-      <c r="F6" s="44" t="s">
+      <c r="F6" s="37" t="s">
         <v>29</v>
       </c>
-      <c r="G6" s="44" t="s">
+      <c r="G6" s="37" t="s">
         <v>30</v>
       </c>
-      <c r="H6" s="46" t="n">
+      <c r="H6" s="39" t="n">
         <v>40294</v>
       </c>
-      <c r="I6" s="46" t="n">
+      <c r="I6" s="39" t="n">
         <v>40294</v>
       </c>
-      <c r="J6" s="46" t="n">
-        <v>43946</v>
-      </c>
-      <c r="K6" s="47" t="n">
+      <c r="J6" s="39" t="n">
+        <v>44676</v>
+      </c>
+      <c r="K6" s="40" t="n">
         <v>1</v>
       </c>
-      <c r="L6" s="44" t="s">
+      <c r="L6" s="37" t="s">
         <v>31</v>
       </c>
-      <c r="M6" s="44" t="s">
+      <c r="M6" s="37" t="s">
         <v>32</v>
       </c>
-      <c r="N6" s="44" t="s">
+      <c r="N6" s="37" t="s">
         <v>33</v>
       </c>
-      <c r="O6" s="44" t="s">
+      <c r="O6" s="37" t="s">
         <v>33</v>
       </c>
-      <c r="P6" s="44" t="s">
+      <c r="P6" s="37" t="s">
         <v>33</v>
       </c>
-      <c r="Q6" s="45" t="s">
+      <c r="Q6" s="38" t="s">
         <v>34</v>
       </c>
-      <c r="R6" s="45" t="s">
+      <c r="R6" s="38" t="s">
         <v>35</v>
       </c>
-      <c r="S6" s="45" t="s">
+      <c r="S6" s="38" t="s">
         <v>36</v>
       </c>
-      <c r="T6" s="45"/>
-      <c r="U6" s="44"/>
-      <c r="V6" s="44"/>
-      <c r="W6" s="44"/>
+      <c r="T6" s="38"/>
+      <c r="U6" s="37"/>
+      <c r="V6" s="37"/>
+      <c r="W6" s="37"/>
     </row>
     <row r="7" s="7" customFormat="true" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A7" s="43" t="n">
+      <c r="A7" s="36" t="n">
         <v>277</v>
       </c>
-      <c r="B7" s="44" t="n">
+      <c r="B7" s="37" t="n">
         <v>1</v>
       </c>
-      <c r="C7" s="45" t="s">
+      <c r="C7" s="38" t="s">
         <v>26</v>
       </c>
-      <c r="D7" s="45" t="s">
+      <c r="D7" s="38" t="s">
         <v>27</v>
       </c>
-      <c r="E7" s="45" t="s">
+      <c r="E7" s="38" t="s">
         <v>28</v>
       </c>
-      <c r="F7" s="44" t="s">
+      <c r="F7" s="37" t="s">
         <v>29</v>
       </c>
-      <c r="G7" s="44" t="s">
+      <c r="G7" s="37" t="s">
         <v>30</v>
       </c>
-      <c r="H7" s="46" t="n">
+      <c r="H7" s="39" t="n">
         <v>40294</v>
       </c>
-      <c r="I7" s="46" t="n">
+      <c r="I7" s="39" t="n">
         <v>40294</v>
       </c>
-      <c r="J7" s="46" t="n">
-        <v>43946</v>
-      </c>
-      <c r="K7" s="47" t="n">
+      <c r="J7" s="39" t="n">
+        <v>44676</v>
+      </c>
+      <c r="K7" s="40" t="n">
         <v>2</v>
       </c>
-      <c r="L7" s="44" t="s">
+      <c r="L7" s="37" t="s">
         <v>37</v>
       </c>
-      <c r="M7" s="44" t="s">
+      <c r="M7" s="37" t="s">
         <v>32</v>
       </c>
-      <c r="N7" s="44" t="s">
+      <c r="N7" s="37" t="s">
         <v>33</v>
       </c>
-      <c r="O7" s="44" t="s">
+      <c r="O7" s="37" t="s">
         <v>33</v>
       </c>
-      <c r="P7" s="44" t="s">
+      <c r="P7" s="37" t="s">
         <v>33</v>
       </c>
-      <c r="Q7" s="45" t="s">
+      <c r="Q7" s="38" t="s">
         <v>34</v>
       </c>
-      <c r="R7" s="45" t="s">
+      <c r="R7" s="38" t="s">
         <v>35</v>
       </c>
-      <c r="S7" s="45" t="s">
+      <c r="S7" s="38" t="s">
         <v>36</v>
       </c>
-      <c r="T7" s="45"/>
-      <c r="U7" s="44"/>
-      <c r="V7" s="44"/>
-      <c r="W7" s="44"/>
+      <c r="T7" s="38"/>
+      <c r="U7" s="37"/>
+      <c r="V7" s="37"/>
+      <c r="W7" s="37"/>
     </row>
     <row r="8" s="7" customFormat="true" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A8" s="43" t="n">
+      <c r="A8" s="36" t="n">
         <v>278</v>
       </c>
-      <c r="B8" s="44" t="n">
+      <c r="B8" s="37" t="n">
         <v>1</v>
       </c>
-      <c r="C8" s="45" t="s">
+      <c r="C8" s="38" t="s">
         <v>38</v>
       </c>
-      <c r="D8" s="45" t="s">
+      <c r="D8" s="38" t="s">
         <v>27</v>
       </c>
-      <c r="E8" s="45" t="s">
+      <c r="E8" s="38" t="s">
         <v>28</v>
       </c>
-      <c r="F8" s="44" t="s">
+      <c r="F8" s="37" t="s">
         <v>29</v>
       </c>
-      <c r="G8" s="44" t="s">
+      <c r="G8" s="37" t="s">
         <v>30</v>
       </c>
-      <c r="H8" s="46" t="n">
+      <c r="H8" s="39" t="n">
         <v>40294</v>
       </c>
-      <c r="I8" s="46" t="n">
+      <c r="I8" s="39" t="n">
         <v>40294</v>
       </c>
-      <c r="J8" s="46" t="n">
+      <c r="J8" s="41" t="n">
         <v>43946</v>
       </c>
-      <c r="K8" s="47" t="n">
+      <c r="K8" s="40" t="n">
         <v>1</v>
       </c>
-      <c r="L8" s="44" t="s">
+      <c r="L8" s="37" t="s">
         <v>31</v>
       </c>
-      <c r="M8" s="44" t="s">
+      <c r="M8" s="37" t="s">
         <v>32</v>
       </c>
-      <c r="N8" s="44" t="s">
+      <c r="N8" s="37" t="s">
         <v>33</v>
       </c>
-      <c r="O8" s="44" t="s">
+      <c r="O8" s="37" t="s">
         <v>33</v>
       </c>
-      <c r="P8" s="44" t="s">
+      <c r="P8" s="37" t="s">
         <v>33</v>
       </c>
-      <c r="Q8" s="45" t="s">
+      <c r="Q8" s="38" t="s">
         <v>39</v>
       </c>
-      <c r="R8" s="45" t="s">
+      <c r="R8" s="38" t="s">
         <v>40</v>
       </c>
-      <c r="S8" s="45" t="s">
+      <c r="S8" s="38" t="s">
         <v>41</v>
       </c>
-      <c r="T8" s="45"/>
-      <c r="U8" s="44"/>
-      <c r="V8" s="44"/>
-      <c r="W8" s="44"/>
+      <c r="T8" s="38"/>
+      <c r="U8" s="37"/>
+      <c r="V8" s="37"/>
+      <c r="W8" s="37"/>
     </row>
     <row r="9" s="7" customFormat="true" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A9" s="48" t="n">
+      <c r="A9" s="42" t="n">
         <v>278</v>
       </c>
-      <c r="B9" s="44" t="n">
+      <c r="B9" s="37" t="n">
         <v>1</v>
       </c>
-      <c r="C9" s="45" t="s">
+      <c r="C9" s="38" t="s">
         <v>38</v>
       </c>
-      <c r="D9" s="45" t="s">
+      <c r="D9" s="38" t="s">
         <v>27</v>
       </c>
-      <c r="E9" s="45" t="s">
+      <c r="E9" s="38" t="s">
         <v>28</v>
       </c>
-      <c r="F9" s="44" t="s">
+      <c r="F9" s="37" t="s">
         <v>29</v>
       </c>
-      <c r="G9" s="44" t="s">
+      <c r="G9" s="37" t="s">
         <v>30</v>
       </c>
-      <c r="H9" s="46" t="n">
+      <c r="H9" s="39" t="n">
         <v>40294</v>
       </c>
-      <c r="I9" s="46" t="n">
+      <c r="I9" s="39" t="n">
         <v>40294</v>
       </c>
-      <c r="J9" s="46" t="n">
+      <c r="J9" s="41" t="n">
         <v>43946</v>
       </c>
-      <c r="K9" s="47" t="n">
+      <c r="K9" s="40" t="n">
         <v>2</v>
       </c>
-      <c r="L9" s="44" t="s">
+      <c r="L9" s="37" t="s">
         <v>37</v>
       </c>
-      <c r="M9" s="44" t="s">
+      <c r="M9" s="37" t="s">
         <v>32</v>
       </c>
-      <c r="N9" s="44" t="s">
+      <c r="N9" s="37" t="s">
         <v>33</v>
       </c>
-      <c r="O9" s="44" t="s">
+      <c r="O9" s="37" t="s">
         <v>33</v>
       </c>
-      <c r="P9" s="44" t="s">
+      <c r="P9" s="37" t="s">
         <v>33</v>
       </c>
-      <c r="Q9" s="45" t="s">
+      <c r="Q9" s="38" t="s">
         <v>39</v>
       </c>
-      <c r="R9" s="45" t="s">
+      <c r="R9" s="38" t="s">
         <v>40</v>
       </c>
-      <c r="S9" s="45" t="s">
+      <c r="S9" s="38" t="s">
         <v>41</v>
       </c>
-      <c r="T9" s="45"/>
-      <c r="U9" s="44"/>
-      <c r="V9" s="44"/>
-      <c r="W9" s="44"/>
+      <c r="T9" s="38"/>
+      <c r="U9" s="37"/>
+      <c r="V9" s="37"/>
+      <c r="W9" s="37"/>
     </row>
-    <row r="10" s="7" customFormat="true" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A10" s="48" t="n">
+    <row r="10" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A10" s="42" t="n">
         <v>279</v>
       </c>
-      <c r="B10" s="49" t="n">
+      <c r="B10" s="43" t="n">
         <v>1</v>
       </c>
-      <c r="C10" s="45" t="s">
+      <c r="C10" s="38" t="s">
         <v>42</v>
       </c>
-      <c r="D10" s="45" t="s">
+      <c r="D10" s="38" t="s">
         <v>27</v>
       </c>
-      <c r="E10" s="45" t="s">
+      <c r="E10" s="38" t="s">
         <v>28</v>
       </c>
-      <c r="F10" s="44" t="s">
+      <c r="F10" s="37" t="s">
         <v>29</v>
       </c>
-      <c r="G10" s="44" t="s">
+      <c r="G10" s="37" t="s">
         <v>30</v>
       </c>
-      <c r="H10" s="46" t="n">
+      <c r="H10" s="39" t="n">
         <v>40294</v>
       </c>
-      <c r="I10" s="46" t="n">
+      <c r="I10" s="39" t="n">
         <v>40294</v>
       </c>
-      <c r="J10" s="46" t="n">
-        <v>43946</v>
-      </c>
-      <c r="K10" s="47" t="n">
+      <c r="J10" s="39" t="n">
+        <v>44676</v>
+      </c>
+      <c r="K10" s="40" t="n">
         <v>1</v>
       </c>
-      <c r="L10" s="44" t="s">
+      <c r="L10" s="37" t="s">
         <v>31</v>
       </c>
-      <c r="M10" s="44" t="s">
+      <c r="M10" s="37" t="s">
         <v>32</v>
       </c>
-      <c r="N10" s="44" t="s">
+      <c r="N10" s="37" t="s">
         <v>33</v>
       </c>
-      <c r="O10" s="44" t="s">
+      <c r="O10" s="37" t="s">
         <v>33</v>
       </c>
-      <c r="P10" s="44" t="s">
+      <c r="P10" s="37" t="s">
         <v>33</v>
       </c>
-      <c r="Q10" s="45" t="s">
+      <c r="Q10" s="38" t="s">
         <v>43</v>
       </c>
-      <c r="R10" s="45" t="s">
+      <c r="R10" s="38" t="s">
         <v>44</v>
       </c>
-      <c r="S10" s="45" t="s">
+      <c r="S10" s="38" t="s">
         <v>41</v>
       </c>
-      <c r="T10" s="45"/>
-      <c r="U10" s="44"/>
-      <c r="V10" s="44"/>
-      <c r="W10" s="44"/>
+      <c r="T10" s="38"/>
+      <c r="U10" s="37"/>
+      <c r="V10" s="37"/>
+      <c r="W10" s="37"/>
     </row>
-    <row r="11" s="7" customFormat="true" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A11" s="48" t="n">
+    <row r="11" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A11" s="42" t="n">
         <v>279</v>
       </c>
-      <c r="B11" s="49" t="n">
+      <c r="B11" s="43" t="n">
         <v>1</v>
       </c>
-      <c r="C11" s="45" t="s">
+      <c r="C11" s="38" t="s">
         <v>42</v>
       </c>
-      <c r="D11" s="45" t="s">
+      <c r="D11" s="38" t="s">
         <v>27</v>
       </c>
-      <c r="E11" s="45" t="s">
+      <c r="E11" s="38" t="s">
         <v>28</v>
       </c>
-      <c r="F11" s="44" t="s">
+      <c r="F11" s="37" t="s">
         <v>29</v>
       </c>
-      <c r="G11" s="44" t="s">
+      <c r="G11" s="37" t="s">
         <v>30</v>
       </c>
-      <c r="H11" s="46" t="n">
+      <c r="H11" s="39" t="n">
         <v>40294</v>
       </c>
-      <c r="I11" s="46" t="n">
+      <c r="I11" s="39" t="n">
         <v>40294</v>
       </c>
-      <c r="J11" s="46" t="n">
-        <v>43946</v>
-      </c>
-      <c r="K11" s="47" t="n">
+      <c r="J11" s="39" t="n">
+        <v>44676</v>
+      </c>
+      <c r="K11" s="40" t="n">
         <v>2</v>
       </c>
-      <c r="L11" s="44" t="s">
+      <c r="L11" s="37" t="s">
         <v>37</v>
       </c>
-      <c r="M11" s="44" t="s">
+      <c r="M11" s="37" t="s">
         <v>32</v>
       </c>
-      <c r="N11" s="44" t="s">
+      <c r="N11" s="37" t="s">
         <v>33</v>
       </c>
-      <c r="O11" s="44" t="s">
+      <c r="O11" s="37" t="s">
         <v>33</v>
       </c>
-      <c r="P11" s="44" t="s">
+      <c r="P11" s="37" t="s">
         <v>33</v>
       </c>
-      <c r="Q11" s="45" t="s">
+      <c r="Q11" s="38" t="s">
         <v>43</v>
       </c>
-      <c r="R11" s="45" t="s">
+      <c r="R11" s="38" t="s">
         <v>44</v>
       </c>
-      <c r="S11" s="45" t="s">
+      <c r="S11" s="38" t="s">
         <v>41</v>
       </c>
-      <c r="T11" s="45"/>
-      <c r="U11" s="44"/>
-      <c r="V11" s="44"/>
-      <c r="W11" s="44"/>
+      <c r="T11" s="38"/>
+      <c r="U11" s="37"/>
+      <c r="V11" s="37"/>
+      <c r="W11" s="37"/>
     </row>
-    <row r="12" s="7" customFormat="true" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A12" s="43" t="n">
+    <row r="12" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A12" s="36" t="n">
         <v>65837</v>
       </c>
-      <c r="B12" s="44" t="n">
+      <c r="B12" s="37" t="n">
         <v>1</v>
       </c>
-      <c r="C12" s="45" t="s">
+      <c r="C12" s="38" t="s">
         <v>45</v>
       </c>
-      <c r="D12" s="45" t="s">
+      <c r="D12" s="38" t="s">
         <v>46</v>
       </c>
-      <c r="E12" s="45" t="s">
+      <c r="E12" s="38" t="s">
         <v>47</v>
       </c>
-      <c r="F12" s="44" t="s">
+      <c r="F12" s="37" t="s">
         <v>48</v>
       </c>
-      <c r="G12" s="44" t="s">
+      <c r="G12" s="37" t="s">
         <v>49</v>
       </c>
-      <c r="H12" s="46" t="n">
+      <c r="H12" s="39" t="n">
         <v>42144</v>
       </c>
-      <c r="I12" s="46" t="n">
+      <c r="I12" s="39" t="n">
         <v>42144</v>
       </c>
-      <c r="J12" s="46" t="n">
+      <c r="J12" s="39" t="n">
         <v>43970</v>
       </c>
-      <c r="K12" s="47" t="n">
+      <c r="K12" s="40" t="n">
         <v>1</v>
       </c>
-      <c r="L12" s="44" t="s">
+      <c r="L12" s="37" t="s">
         <v>50</v>
       </c>
-      <c r="M12" s="44" t="s">
+      <c r="M12" s="37" t="s">
         <v>51</v>
       </c>
-      <c r="N12" s="44" t="s">
+      <c r="N12" s="37" t="s">
         <v>52</v>
       </c>
-      <c r="O12" s="44" t="s">
+      <c r="O12" s="37" t="s">
         <v>52</v>
       </c>
-      <c r="P12" s="44" t="s">
+      <c r="P12" s="37" t="s">
         <v>52</v>
       </c>
-      <c r="Q12" s="45" t="s">
+      <c r="Q12" s="38" t="s">
         <v>53</v>
       </c>
-      <c r="R12" s="45" t="s">
+      <c r="R12" s="38" t="s">
         <v>54</v>
       </c>
-      <c r="S12" s="45" t="s">
+      <c r="S12" s="38" t="s">
         <v>55</v>
       </c>
-      <c r="T12" s="45"/>
-      <c r="U12" s="44"/>
-      <c r="V12" s="44"/>
-      <c r="W12" s="44"/>
+      <c r="T12" s="38"/>
+      <c r="U12" s="37"/>
+      <c r="V12" s="37"/>
+      <c r="W12" s="37"/>
     </row>
-    <row r="13" s="7" customFormat="true" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A13" s="43" t="n">
+    <row r="13" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A13" s="36" t="n">
         <v>65838</v>
       </c>
-      <c r="B13" s="44" t="n">
+      <c r="B13" s="37" t="n">
         <v>1</v>
       </c>
-      <c r="C13" s="45" t="s">
+      <c r="C13" s="38" t="s">
         <v>56</v>
       </c>
-      <c r="D13" s="45" t="s">
+      <c r="D13" s="38" t="s">
         <v>57</v>
       </c>
-      <c r="E13" s="45" t="s">
+      <c r="E13" s="38" t="s">
         <v>58</v>
       </c>
-      <c r="F13" s="44" t="s">
+      <c r="F13" s="37" t="s">
         <v>59</v>
       </c>
-      <c r="G13" s="44" t="s">
+      <c r="G13" s="37" t="s">
         <v>60</v>
       </c>
-      <c r="H13" s="46" t="n">
+      <c r="H13" s="39" t="n">
         <v>42159</v>
       </c>
-      <c r="I13" s="46" t="n">
+      <c r="I13" s="39" t="n">
         <v>42159</v>
       </c>
-      <c r="J13" s="46" t="n">
+      <c r="J13" s="39" t="n">
         <v>43985</v>
       </c>
-      <c r="K13" s="47" t="n">
+      <c r="K13" s="40" t="n">
         <v>3</v>
       </c>
-      <c r="L13" s="44" t="s">
+      <c r="L13" s="37" t="s">
         <v>61</v>
       </c>
-      <c r="M13" s="44" t="s">
+      <c r="M13" s="37" t="s">
         <v>62</v>
       </c>
-      <c r="N13" s="44" t="s">
+      <c r="N13" s="37" t="s">
         <v>63</v>
       </c>
-      <c r="O13" s="44" t="s">
+      <c r="O13" s="37" t="s">
         <v>63</v>
       </c>
-      <c r="P13" s="44" t="s">
+      <c r="P13" s="37" t="s">
         <v>63</v>
       </c>
-      <c r="Q13" s="45" t="s">
+      <c r="Q13" s="38" t="s">
         <v>64</v>
       </c>
-      <c r="R13" s="45" t="s">
+      <c r="R13" s="38" t="s">
         <v>65</v>
       </c>
-      <c r="S13" s="45" t="s">
+      <c r="S13" s="38" t="s">
         <v>66</v>
       </c>
-      <c r="T13" s="45"/>
-      <c r="U13" s="44"/>
-      <c r="V13" s="44"/>
-      <c r="W13" s="44"/>
+      <c r="T13" s="38"/>
+      <c r="U13" s="37"/>
+      <c r="V13" s="37"/>
+      <c r="W13" s="37"/>
     </row>
     <row r="5574" customFormat="false" ht="24" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
   </sheetData>
@@ -4405,7 +4364,7 @@
   </mergeCells>
   <printOptions headings="false" gridLines="true" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.340277777777778" right="0" top="0.275694444444444" bottom="0.472222222222222" header="0.511805555555555" footer="0.0784722222222222"/>
-  <pageSetup paperSize="8" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="overThenDown" orientation="landscape" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="8" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="overThenDown" orientation="landscape" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader/>
     <oddFooter>&amp;C&amp;9Swissmedic · Hallerstrasse 7 · CH-3000 Bern 9 · www.swissmedic.ch · Tel. +41 58 462 02 11 · Fax +41 58 462 02 12&amp;R&amp;9&amp;P/&amp;N</oddFooter>

</xml_diff>

<commit_message>
(#3) Set date to nil when expiration_date is a string 'Unbegrenzt'
</commit_message>
<xml_diff>
--- a/test/data/Packungen-2015.07.02.xlsx
+++ b/test/data/Packungen-2015.07.02.xlsx
@@ -14,6 +14,7 @@
     <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Titles" vbProcedure="false">'Zugelassene Packungen'!$5:$5</definedName>
     <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Titles" vbProcedure="false">'Zugelassene Packungen'!$5:$5</definedName>
     <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Titles_0" vbProcedure="false">'Zugelassene Packungen'!$5:$5</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Titles_0_0" vbProcedure="false">'Zugelassene Packungen'!$5:$5</definedName>
   </definedNames>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
   <extLst>
@@ -25,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="130" uniqueCount="67">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="144" uniqueCount="76">
   <si>
     <t xml:space="preserve">Zugelassene Packungen / Conditionnements autorisés</t>
   </si>
@@ -286,6 +287,33 @@
   </si>
   <si>
     <t xml:space="preserve">Bei kleineren Hautverletzungen</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Zymafluor 0.25 mg, Tabletten</t>
+  </si>
+  <si>
+    <t xml:space="preserve">MEDA Pharma GmbH</t>
+  </si>
+  <si>
+    <t xml:space="preserve">13.05.1.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">A01AA01</t>
+  </si>
+  <si>
+    <t xml:space="preserve">unbegrenzt</t>
+  </si>
+  <si>
+    <t xml:space="preserve">400</t>
+  </si>
+  <si>
+    <t xml:space="preserve">fluoridum</t>
+  </si>
+  <si>
+    <t xml:space="preserve">fluoridum 0.25 mg ut natrii fluoridum, aromatica, excipiens pro compresso.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Kariesprophylaxe</t>
   </si>
 </sst>
 </file>
@@ -611,13 +639,13 @@
     </xf>
   </cellXfs>
   <cellStyles count="7">
-    <cellStyle name="Normal" xfId="0" builtinId="0" customBuiltin="false"/>
-    <cellStyle name="Comma" xfId="15" builtinId="3" customBuiltin="false"/>
-    <cellStyle name="Comma [0]" xfId="16" builtinId="6" customBuiltin="false"/>
-    <cellStyle name="Currency" xfId="17" builtinId="4" customBuiltin="false"/>
-    <cellStyle name="Currency [0]" xfId="18" builtinId="7" customBuiltin="false"/>
-    <cellStyle name="Percent" xfId="19" builtinId="5" customBuiltin="false"/>
-    <cellStyle name="Excel Built-in Standard 2" xfId="20" builtinId="53" customBuiltin="true"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Comma" xfId="15" builtinId="3"/>
+    <cellStyle name="Comma [0]" xfId="16" builtinId="6"/>
+    <cellStyle name="Currency" xfId="17" builtinId="4"/>
+    <cellStyle name="Currency [0]" xfId="18" builtinId="7"/>
+    <cellStyle name="Percent" xfId="19" builtinId="5"/>
+    <cellStyle name="Excel Built-in Explanatory Text" xfId="20"/>
   </cellStyles>
 </styleSheet>
 </file>
@@ -633,9 +661,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>2</xdr:col>
-      <xdr:colOff>360000</xdr:colOff>
+      <xdr:colOff>359640</xdr:colOff>
       <xdr:row>1</xdr:row>
-      <xdr:rowOff>238320</xdr:rowOff>
+      <xdr:rowOff>237960</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -649,7 +677,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="36360" y="360"/>
-          <a:ext cx="1600560" cy="504360"/>
+          <a:ext cx="1600560" cy="504000"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -674,19 +702,19 @@
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="false" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="0" ySplit="5" topLeftCell="A6" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="J9" activeCellId="0" sqref="J9"/>
+      <selection pane="bottomLeft" activeCell="A14" activeCellId="0" sqref="A14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.75" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="9.12"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="2" width="7.38"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="2" width="7.39"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="3" width="33.87"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="3" width="23"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="3" width="15.87"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="2" width="7.87"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="2" width="8.12"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="8" style="4" width="10.26"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="8" style="4" width="10.27"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="4" width="10.13"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="4" width="9.26"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="2" width="11"/>
@@ -695,12 +723,12 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="15" min="15" style="6" width="10.38"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="16" min="16" style="2" width="10.38"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="18" min="17" style="3" width="22.13"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="20" min="19" style="3" width="26.38"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="20" min="19" style="3" width="26.39"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="22" min="21" style="2" width="16.13"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="23" min="23" style="2" width="14.13"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="24" min="24" style="0" width="8.61"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="24" min="24" style="0" width="8.6"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="27" min="25" style="7" width="7.25"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="28" min="28" style="7" width="8.38"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="28" min="28" style="7" width="8.39"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="29" min="29" style="7" width="7.25"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="30" min="30" style="7" width="14.25"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="31" min="31" style="7" width="7.25"/>
@@ -4357,6 +4385,70 @@
       <c r="V13" s="37"/>
       <c r="W13" s="37"/>
     </row>
+    <row r="14" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A14" s="36" t="n">
+        <v>15219</v>
+      </c>
+      <c r="B14" s="37" t="n">
+        <v>1</v>
+      </c>
+      <c r="C14" s="38" t="s">
+        <v>67</v>
+      </c>
+      <c r="D14" s="38" t="s">
+        <v>68</v>
+      </c>
+      <c r="E14" s="38" t="s">
+        <v>47</v>
+      </c>
+      <c r="F14" s="37" t="s">
+        <v>69</v>
+      </c>
+      <c r="G14" s="37" t="s">
+        <v>70</v>
+      </c>
+      <c r="H14" s="39" t="n">
+        <v>18429</v>
+      </c>
+      <c r="I14" s="39" t="n">
+        <v>18429</v>
+      </c>
+      <c r="J14" s="39" t="s">
+        <v>71</v>
+      </c>
+      <c r="K14" s="40" t="n">
+        <v>68</v>
+      </c>
+      <c r="L14" s="37" t="s">
+        <v>72</v>
+      </c>
+      <c r="M14" s="37" t="s">
+        <v>51</v>
+      </c>
+      <c r="N14" s="37" t="s">
+        <v>52</v>
+      </c>
+      <c r="O14" s="37" t="s">
+        <v>52</v>
+      </c>
+      <c r="P14" s="37" t="s">
+        <v>52</v>
+      </c>
+      <c r="Q14" s="38" t="s">
+        <v>73</v>
+      </c>
+      <c r="R14" s="38" t="s">
+        <v>74</v>
+      </c>
+      <c r="S14" s="38"/>
+      <c r="T14" s="38" t="s">
+        <v>75</v>
+      </c>
+      <c r="U14" s="38"/>
+      <c r="V14" s="37"/>
+      <c r="W14" s="37"/>
+      <c r="X14" s="37"/>
+    </row>
     <row r="5574" customFormat="false" ht="24" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
   </sheetData>
   <mergeCells count="1">

</xml_diff>